<commit_message>
Atualizado lisks redes sociais
</commit_message>
<xml_diff>
--- a/Gráfico de Gantt.xlsx
+++ b/Gráfico de Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" backupFile="1" codeName="EstaPastaDeTrabalho"/>
-  <xr:revisionPtr revIDLastSave="934" documentId="8_{4EC56E9F-A59D-435C-9260-10A796BED726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F586377-7458-47D8-9F01-A3D77CFD0584}"/>
+  <xr:revisionPtr revIDLastSave="945" documentId="8_{4EC56E9F-A59D-435C-9260-10A796BED726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB22F8D3-7D04-4813-A12F-2EC68A0E3021}"/>
   <bookViews>
     <workbookView showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="0" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3478" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3479" uniqueCount="117">
   <si>
     <t>Insira o Nome da empresa na célula B2.</t>
   </si>
@@ -621,6 +621,9 @@
       <t>👍</t>
     </r>
   </si>
+  <si>
+    <t>GitHub</t>
+  </si>
 </sst>
 </file>
 
@@ -1041,7 +1044,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="63">
+  <fills count="65">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1397,6 +1400,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF6969"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2178,7 +2193,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -2797,16 +2812,19 @@
     <xf numFmtId="168" fontId="6" fillId="0" borderId="30" xfId="9" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="45" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="46" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2815,17 +2833,14 @@
     <xf numFmtId="0" fontId="47" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="50" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="50" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2912,6 +2927,14 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="60" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="64" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="63" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
@@ -6182,7 +6205,7 @@
         <xdr:cNvPr id="3" name="Balão de Fala: Retângulo com Cantos Arredondados 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AD308B7-C7EB-29D4-1DE0-54EDFD9F5965}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8031,6 +8054,7 @@
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="21" name="Imagem 20">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000015000000}"/>
@@ -8042,7 +8066,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -8081,6 +8105,7 @@
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="23" name="Imagem 22">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000017000000}"/>
@@ -8092,7 +8117,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -8107,6 +8132,57 @@
         <a:xfrm>
           <a:off x="381000" y="2343150"/>
           <a:ext cx="1257071" cy="1257071"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>209398</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142723</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3848100" y="2409825"/>
+          <a:ext cx="1219048" cy="1219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13052,9 +13128,9 @@
   </sheetPr>
   <dimension ref="A1:CD251"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -35580,1076 +35656,1092 @@
     <row r="1" spans="1:34" ht="90.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="191" t="s">
+      <c r="A3" s="184" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="191"/>
-      <c r="C3" s="191"/>
-      <c r="D3" s="191"/>
-      <c r="E3" s="191"/>
-      <c r="F3" s="191"/>
-      <c r="H3" s="186" t="s">
+      <c r="B3" s="184"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="184"/>
+      <c r="H3" s="187" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="186"/>
-      <c r="J3" s="186"/>
-      <c r="K3" s="186"/>
-      <c r="L3" s="186"/>
-      <c r="M3" s="186"/>
-      <c r="O3" s="187" t="s">
+      <c r="I3" s="187"/>
+      <c r="J3" s="187"/>
+      <c r="K3" s="187"/>
+      <c r="L3" s="187"/>
+      <c r="M3" s="187"/>
+      <c r="O3" s="188" t="s">
         <v>64</v>
       </c>
-      <c r="P3" s="187"/>
-      <c r="Q3" s="187"/>
-      <c r="R3" s="187"/>
-      <c r="S3" s="187"/>
-      <c r="T3" s="187"/>
-      <c r="V3" s="188" t="s">
+      <c r="P3" s="188"/>
+      <c r="Q3" s="188"/>
+      <c r="R3" s="188"/>
+      <c r="S3" s="188"/>
+      <c r="T3" s="188"/>
+      <c r="V3" s="185" t="s">
         <v>64</v>
       </c>
-      <c r="W3" s="188"/>
-      <c r="X3" s="188"/>
-      <c r="Y3" s="188"/>
-      <c r="Z3" s="188"/>
-      <c r="AA3" s="188"/>
-      <c r="AC3" s="189" t="s">
+      <c r="W3" s="185"/>
+      <c r="X3" s="185"/>
+      <c r="Y3" s="185"/>
+      <c r="Z3" s="185"/>
+      <c r="AA3" s="185"/>
+      <c r="AC3" s="182" t="s">
         <v>64</v>
       </c>
-      <c r="AD3" s="189"/>
-      <c r="AE3" s="189"/>
-      <c r="AF3" s="189"/>
-      <c r="AG3" s="189"/>
-      <c r="AH3" s="189"/>
+      <c r="AD3" s="182"/>
+      <c r="AE3" s="182"/>
+      <c r="AF3" s="182"/>
+      <c r="AG3" s="182"/>
+      <c r="AH3" s="182"/>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="190" t="s">
+      <c r="A4" s="189" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="190"/>
-      <c r="C4" s="190"/>
-      <c r="D4" s="190"/>
-      <c r="E4" s="190"/>
-      <c r="F4" s="190"/>
-      <c r="H4" s="182" t="s">
+      <c r="B4" s="189"/>
+      <c r="C4" s="189"/>
+      <c r="D4" s="189"/>
+      <c r="E4" s="189"/>
+      <c r="F4" s="189"/>
+      <c r="H4" s="190" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="182"/>
-      <c r="J4" s="182"/>
-      <c r="K4" s="182"/>
-      <c r="L4" s="182"/>
-      <c r="M4" s="182"/>
-      <c r="O4" s="183" t="s">
+      <c r="I4" s="190"/>
+      <c r="J4" s="190"/>
+      <c r="K4" s="190"/>
+      <c r="L4" s="190"/>
+      <c r="M4" s="190"/>
+      <c r="O4" s="191" t="s">
         <v>65</v>
       </c>
-      <c r="P4" s="183"/>
-      <c r="Q4" s="183"/>
-      <c r="R4" s="183"/>
-      <c r="S4" s="183"/>
-      <c r="T4" s="183"/>
-      <c r="V4" s="184" t="s">
+      <c r="P4" s="191"/>
+      <c r="Q4" s="191"/>
+      <c r="R4" s="191"/>
+      <c r="S4" s="191"/>
+      <c r="T4" s="191"/>
+      <c r="V4" s="186" t="s">
         <v>65</v>
       </c>
-      <c r="W4" s="184"/>
-      <c r="X4" s="184"/>
-      <c r="Y4" s="184"/>
-      <c r="Z4" s="184"/>
-      <c r="AA4" s="184"/>
-      <c r="AC4" s="185" t="s">
+      <c r="W4" s="186"/>
+      <c r="X4" s="186"/>
+      <c r="Y4" s="186"/>
+      <c r="Z4" s="186"/>
+      <c r="AA4" s="186"/>
+      <c r="AC4" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="AD4" s="185"/>
-      <c r="AE4" s="185"/>
-      <c r="AF4" s="185"/>
-      <c r="AG4" s="185"/>
-      <c r="AH4" s="185"/>
+      <c r="AD4" s="183"/>
+      <c r="AE4" s="183"/>
+      <c r="AF4" s="183"/>
+      <c r="AG4" s="183"/>
+      <c r="AH4" s="183"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A5" s="190"/>
-      <c r="B5" s="190"/>
-      <c r="C5" s="190"/>
-      <c r="D5" s="190"/>
-      <c r="E5" s="190"/>
-      <c r="F5" s="190"/>
-      <c r="H5" s="182"/>
-      <c r="I5" s="182"/>
-      <c r="J5" s="182"/>
-      <c r="K5" s="182"/>
-      <c r="L5" s="182"/>
-      <c r="M5" s="182"/>
-      <c r="O5" s="183"/>
-      <c r="P5" s="183"/>
-      <c r="Q5" s="183"/>
-      <c r="R5" s="183"/>
-      <c r="S5" s="183"/>
-      <c r="T5" s="183"/>
-      <c r="V5" s="184"/>
-      <c r="W5" s="184"/>
-      <c r="X5" s="184"/>
-      <c r="Y5" s="184"/>
-      <c r="Z5" s="184"/>
-      <c r="AA5" s="184"/>
-      <c r="AC5" s="185"/>
-      <c r="AD5" s="185"/>
-      <c r="AE5" s="185"/>
-      <c r="AF5" s="185"/>
-      <c r="AG5" s="185"/>
-      <c r="AH5" s="185"/>
+      <c r="A5" s="189"/>
+      <c r="B5" s="189"/>
+      <c r="C5" s="189"/>
+      <c r="D5" s="189"/>
+      <c r="E5" s="189"/>
+      <c r="F5" s="189"/>
+      <c r="H5" s="190"/>
+      <c r="I5" s="190"/>
+      <c r="J5" s="190"/>
+      <c r="K5" s="190"/>
+      <c r="L5" s="190"/>
+      <c r="M5" s="190"/>
+      <c r="O5" s="191"/>
+      <c r="P5" s="191"/>
+      <c r="Q5" s="191"/>
+      <c r="R5" s="191"/>
+      <c r="S5" s="191"/>
+      <c r="T5" s="191"/>
+      <c r="V5" s="186"/>
+      <c r="W5" s="186"/>
+      <c r="X5" s="186"/>
+      <c r="Y5" s="186"/>
+      <c r="Z5" s="186"/>
+      <c r="AA5" s="186"/>
+      <c r="AC5" s="183"/>
+      <c r="AD5" s="183"/>
+      <c r="AE5" s="183"/>
+      <c r="AF5" s="183"/>
+      <c r="AG5" s="183"/>
+      <c r="AH5" s="183"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6" s="190"/>
-      <c r="B6" s="190"/>
-      <c r="C6" s="190"/>
-      <c r="D6" s="190"/>
-      <c r="E6" s="190"/>
-      <c r="F6" s="190"/>
-      <c r="H6" s="182"/>
-      <c r="I6" s="182"/>
-      <c r="J6" s="182"/>
-      <c r="K6" s="182"/>
-      <c r="L6" s="182"/>
-      <c r="M6" s="182"/>
-      <c r="O6" s="183"/>
-      <c r="P6" s="183"/>
-      <c r="Q6" s="183"/>
-      <c r="R6" s="183"/>
-      <c r="S6" s="183"/>
-      <c r="T6" s="183"/>
-      <c r="V6" s="184"/>
-      <c r="W6" s="184"/>
-      <c r="X6" s="184"/>
-      <c r="Y6" s="184"/>
-      <c r="Z6" s="184"/>
-      <c r="AA6" s="184"/>
-      <c r="AC6" s="185"/>
-      <c r="AD6" s="185"/>
-      <c r="AE6" s="185"/>
-      <c r="AF6" s="185"/>
-      <c r="AG6" s="185"/>
-      <c r="AH6" s="185"/>
+      <c r="A6" s="189"/>
+      <c r="B6" s="189"/>
+      <c r="C6" s="189"/>
+      <c r="D6" s="189"/>
+      <c r="E6" s="189"/>
+      <c r="F6" s="189"/>
+      <c r="H6" s="190"/>
+      <c r="I6" s="190"/>
+      <c r="J6" s="190"/>
+      <c r="K6" s="190"/>
+      <c r="L6" s="190"/>
+      <c r="M6" s="190"/>
+      <c r="O6" s="191"/>
+      <c r="P6" s="191"/>
+      <c r="Q6" s="191"/>
+      <c r="R6" s="191"/>
+      <c r="S6" s="191"/>
+      <c r="T6" s="191"/>
+      <c r="V6" s="186"/>
+      <c r="W6" s="186"/>
+      <c r="X6" s="186"/>
+      <c r="Y6" s="186"/>
+      <c r="Z6" s="186"/>
+      <c r="AA6" s="186"/>
+      <c r="AC6" s="183"/>
+      <c r="AD6" s="183"/>
+      <c r="AE6" s="183"/>
+      <c r="AF6" s="183"/>
+      <c r="AG6" s="183"/>
+      <c r="AH6" s="183"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" s="190"/>
-      <c r="B7" s="190"/>
-      <c r="C7" s="190"/>
-      <c r="D7" s="190"/>
-      <c r="E7" s="190"/>
-      <c r="F7" s="190"/>
-      <c r="H7" s="182"/>
-      <c r="I7" s="182"/>
-      <c r="J7" s="182"/>
-      <c r="K7" s="182"/>
-      <c r="L7" s="182"/>
-      <c r="M7" s="182"/>
-      <c r="O7" s="183"/>
-      <c r="P7" s="183"/>
-      <c r="Q7" s="183"/>
-      <c r="R7" s="183"/>
-      <c r="S7" s="183"/>
-      <c r="T7" s="183"/>
-      <c r="V7" s="184"/>
-      <c r="W7" s="184"/>
-      <c r="X7" s="184"/>
-      <c r="Y7" s="184"/>
-      <c r="Z7" s="184"/>
-      <c r="AA7" s="184"/>
-      <c r="AC7" s="185"/>
-      <c r="AD7" s="185"/>
-      <c r="AE7" s="185"/>
-      <c r="AF7" s="185"/>
-      <c r="AG7" s="185"/>
-      <c r="AH7" s="185"/>
+      <c r="A7" s="189"/>
+      <c r="B7" s="189"/>
+      <c r="C7" s="189"/>
+      <c r="D7" s="189"/>
+      <c r="E7" s="189"/>
+      <c r="F7" s="189"/>
+      <c r="H7" s="190"/>
+      <c r="I7" s="190"/>
+      <c r="J7" s="190"/>
+      <c r="K7" s="190"/>
+      <c r="L7" s="190"/>
+      <c r="M7" s="190"/>
+      <c r="O7" s="191"/>
+      <c r="P7" s="191"/>
+      <c r="Q7" s="191"/>
+      <c r="R7" s="191"/>
+      <c r="S7" s="191"/>
+      <c r="T7" s="191"/>
+      <c r="V7" s="186"/>
+      <c r="W7" s="186"/>
+      <c r="X7" s="186"/>
+      <c r="Y7" s="186"/>
+      <c r="Z7" s="186"/>
+      <c r="AA7" s="186"/>
+      <c r="AC7" s="183"/>
+      <c r="AD7" s="183"/>
+      <c r="AE7" s="183"/>
+      <c r="AF7" s="183"/>
+      <c r="AG7" s="183"/>
+      <c r="AH7" s="183"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" s="190"/>
-      <c r="B8" s="190"/>
-      <c r="C8" s="190"/>
-      <c r="D8" s="190"/>
-      <c r="E8" s="190"/>
-      <c r="F8" s="190"/>
-      <c r="H8" s="182"/>
-      <c r="I8" s="182"/>
-      <c r="J8" s="182"/>
-      <c r="K8" s="182"/>
-      <c r="L8" s="182"/>
-      <c r="M8" s="182"/>
-      <c r="O8" s="183"/>
-      <c r="P8" s="183"/>
-      <c r="Q8" s="183"/>
-      <c r="R8" s="183"/>
-      <c r="S8" s="183"/>
-      <c r="T8" s="183"/>
-      <c r="V8" s="184"/>
-      <c r="W8" s="184"/>
-      <c r="X8" s="184"/>
-      <c r="Y8" s="184"/>
-      <c r="Z8" s="184"/>
-      <c r="AA8" s="184"/>
-      <c r="AC8" s="185"/>
-      <c r="AD8" s="185"/>
-      <c r="AE8" s="185"/>
-      <c r="AF8" s="185"/>
-      <c r="AG8" s="185"/>
-      <c r="AH8" s="185"/>
+      <c r="A8" s="189"/>
+      <c r="B8" s="189"/>
+      <c r="C8" s="189"/>
+      <c r="D8" s="189"/>
+      <c r="E8" s="189"/>
+      <c r="F8" s="189"/>
+      <c r="H8" s="190"/>
+      <c r="I8" s="190"/>
+      <c r="J8" s="190"/>
+      <c r="K8" s="190"/>
+      <c r="L8" s="190"/>
+      <c r="M8" s="190"/>
+      <c r="O8" s="191"/>
+      <c r="P8" s="191"/>
+      <c r="Q8" s="191"/>
+      <c r="R8" s="191"/>
+      <c r="S8" s="191"/>
+      <c r="T8" s="191"/>
+      <c r="V8" s="186"/>
+      <c r="W8" s="186"/>
+      <c r="X8" s="186"/>
+      <c r="Y8" s="186"/>
+      <c r="Z8" s="186"/>
+      <c r="AA8" s="186"/>
+      <c r="AC8" s="183"/>
+      <c r="AD8" s="183"/>
+      <c r="AE8" s="183"/>
+      <c r="AF8" s="183"/>
+      <c r="AG8" s="183"/>
+      <c r="AH8" s="183"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="191" t="s">
+      <c r="A10" s="184" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="191"/>
-      <c r="C10" s="191"/>
-      <c r="D10" s="191"/>
-      <c r="E10" s="191"/>
-      <c r="F10" s="191"/>
-      <c r="H10" s="186" t="s">
+      <c r="B10" s="184"/>
+      <c r="C10" s="184"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="H10" s="187" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="186"/>
-      <c r="J10" s="186"/>
-      <c r="K10" s="186"/>
-      <c r="L10" s="186"/>
-      <c r="M10" s="186"/>
-      <c r="O10" s="187" t="s">
+      <c r="I10" s="187"/>
+      <c r="J10" s="187"/>
+      <c r="K10" s="187"/>
+      <c r="L10" s="187"/>
+      <c r="M10" s="187"/>
+      <c r="O10" s="188" t="s">
         <v>64</v>
       </c>
-      <c r="P10" s="187"/>
-      <c r="Q10" s="187"/>
-      <c r="R10" s="187"/>
-      <c r="S10" s="187"/>
-      <c r="T10" s="187"/>
-      <c r="V10" s="188" t="s">
+      <c r="P10" s="188"/>
+      <c r="Q10" s="188"/>
+      <c r="R10" s="188"/>
+      <c r="S10" s="188"/>
+      <c r="T10" s="188"/>
+      <c r="V10" s="185" t="s">
         <v>64</v>
       </c>
-      <c r="W10" s="188"/>
-      <c r="X10" s="188"/>
-      <c r="Y10" s="188"/>
-      <c r="Z10" s="188"/>
-      <c r="AA10" s="188"/>
-      <c r="AC10" s="189" t="s">
+      <c r="W10" s="185"/>
+      <c r="X10" s="185"/>
+      <c r="Y10" s="185"/>
+      <c r="Z10" s="185"/>
+      <c r="AA10" s="185"/>
+      <c r="AC10" s="182" t="s">
         <v>64</v>
       </c>
-      <c r="AD10" s="189"/>
-      <c r="AE10" s="189"/>
-      <c r="AF10" s="189"/>
-      <c r="AG10" s="189"/>
-      <c r="AH10" s="189"/>
+      <c r="AD10" s="182"/>
+      <c r="AE10" s="182"/>
+      <c r="AF10" s="182"/>
+      <c r="AG10" s="182"/>
+      <c r="AH10" s="182"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" s="190" t="s">
+      <c r="A11" s="189" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="190"/>
-      <c r="C11" s="190"/>
-      <c r="D11" s="190"/>
-      <c r="E11" s="190"/>
-      <c r="F11" s="190"/>
-      <c r="H11" s="182" t="s">
+      <c r="B11" s="189"/>
+      <c r="C11" s="189"/>
+      <c r="D11" s="189"/>
+      <c r="E11" s="189"/>
+      <c r="F11" s="189"/>
+      <c r="H11" s="190" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="182"/>
-      <c r="J11" s="182"/>
-      <c r="K11" s="182"/>
-      <c r="L11" s="182"/>
-      <c r="M11" s="182"/>
-      <c r="O11" s="183" t="s">
+      <c r="I11" s="190"/>
+      <c r="J11" s="190"/>
+      <c r="K11" s="190"/>
+      <c r="L11" s="190"/>
+      <c r="M11" s="190"/>
+      <c r="O11" s="191" t="s">
         <v>65</v>
       </c>
-      <c r="P11" s="183"/>
-      <c r="Q11" s="183"/>
-      <c r="R11" s="183"/>
-      <c r="S11" s="183"/>
-      <c r="T11" s="183"/>
-      <c r="V11" s="184" t="s">
+      <c r="P11" s="191"/>
+      <c r="Q11" s="191"/>
+      <c r="R11" s="191"/>
+      <c r="S11" s="191"/>
+      <c r="T11" s="191"/>
+      <c r="V11" s="186" t="s">
         <v>65</v>
       </c>
-      <c r="W11" s="184"/>
-      <c r="X11" s="184"/>
-      <c r="Y11" s="184"/>
-      <c r="Z11" s="184"/>
-      <c r="AA11" s="184"/>
-      <c r="AC11" s="185" t="s">
+      <c r="W11" s="186"/>
+      <c r="X11" s="186"/>
+      <c r="Y11" s="186"/>
+      <c r="Z11" s="186"/>
+      <c r="AA11" s="186"/>
+      <c r="AC11" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="AD11" s="185"/>
-      <c r="AE11" s="185"/>
-      <c r="AF11" s="185"/>
-      <c r="AG11" s="185"/>
-      <c r="AH11" s="185"/>
+      <c r="AD11" s="183"/>
+      <c r="AE11" s="183"/>
+      <c r="AF11" s="183"/>
+      <c r="AG11" s="183"/>
+      <c r="AH11" s="183"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" s="190"/>
-      <c r="B12" s="190"/>
-      <c r="C12" s="190"/>
-      <c r="D12" s="190"/>
-      <c r="E12" s="190"/>
-      <c r="F12" s="190"/>
-      <c r="H12" s="182"/>
-      <c r="I12" s="182"/>
-      <c r="J12" s="182"/>
-      <c r="K12" s="182"/>
-      <c r="L12" s="182"/>
-      <c r="M12" s="182"/>
-      <c r="O12" s="183"/>
-      <c r="P12" s="183"/>
-      <c r="Q12" s="183"/>
-      <c r="R12" s="183"/>
-      <c r="S12" s="183"/>
-      <c r="T12" s="183"/>
-      <c r="V12" s="184"/>
-      <c r="W12" s="184"/>
-      <c r="X12" s="184"/>
-      <c r="Y12" s="184"/>
-      <c r="Z12" s="184"/>
-      <c r="AA12" s="184"/>
-      <c r="AC12" s="185"/>
-      <c r="AD12" s="185"/>
-      <c r="AE12" s="185"/>
-      <c r="AF12" s="185"/>
-      <c r="AG12" s="185"/>
-      <c r="AH12" s="185"/>
+      <c r="A12" s="189"/>
+      <c r="B12" s="189"/>
+      <c r="C12" s="189"/>
+      <c r="D12" s="189"/>
+      <c r="E12" s="189"/>
+      <c r="F12" s="189"/>
+      <c r="H12" s="190"/>
+      <c r="I12" s="190"/>
+      <c r="J12" s="190"/>
+      <c r="K12" s="190"/>
+      <c r="L12" s="190"/>
+      <c r="M12" s="190"/>
+      <c r="O12" s="191"/>
+      <c r="P12" s="191"/>
+      <c r="Q12" s="191"/>
+      <c r="R12" s="191"/>
+      <c r="S12" s="191"/>
+      <c r="T12" s="191"/>
+      <c r="V12" s="186"/>
+      <c r="W12" s="186"/>
+      <c r="X12" s="186"/>
+      <c r="Y12" s="186"/>
+      <c r="Z12" s="186"/>
+      <c r="AA12" s="186"/>
+      <c r="AC12" s="183"/>
+      <c r="AD12" s="183"/>
+      <c r="AE12" s="183"/>
+      <c r="AF12" s="183"/>
+      <c r="AG12" s="183"/>
+      <c r="AH12" s="183"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="190"/>
-      <c r="B13" s="190"/>
-      <c r="C13" s="190"/>
-      <c r="D13" s="190"/>
-      <c r="E13" s="190"/>
-      <c r="F13" s="190"/>
-      <c r="H13" s="182"/>
-      <c r="I13" s="182"/>
-      <c r="J13" s="182"/>
-      <c r="K13" s="182"/>
-      <c r="L13" s="182"/>
-      <c r="M13" s="182"/>
-      <c r="O13" s="183"/>
-      <c r="P13" s="183"/>
-      <c r="Q13" s="183"/>
-      <c r="R13" s="183"/>
-      <c r="S13" s="183"/>
-      <c r="T13" s="183"/>
-      <c r="V13" s="184"/>
-      <c r="W13" s="184"/>
-      <c r="X13" s="184"/>
-      <c r="Y13" s="184"/>
-      <c r="Z13" s="184"/>
-      <c r="AA13" s="184"/>
-      <c r="AC13" s="185"/>
-      <c r="AD13" s="185"/>
-      <c r="AE13" s="185"/>
-      <c r="AF13" s="185"/>
-      <c r="AG13" s="185"/>
-      <c r="AH13" s="185"/>
+      <c r="A13" s="189"/>
+      <c r="B13" s="189"/>
+      <c r="C13" s="189"/>
+      <c r="D13" s="189"/>
+      <c r="E13" s="189"/>
+      <c r="F13" s="189"/>
+      <c r="H13" s="190"/>
+      <c r="I13" s="190"/>
+      <c r="J13" s="190"/>
+      <c r="K13" s="190"/>
+      <c r="L13" s="190"/>
+      <c r="M13" s="190"/>
+      <c r="O13" s="191"/>
+      <c r="P13" s="191"/>
+      <c r="Q13" s="191"/>
+      <c r="R13" s="191"/>
+      <c r="S13" s="191"/>
+      <c r="T13" s="191"/>
+      <c r="V13" s="186"/>
+      <c r="W13" s="186"/>
+      <c r="X13" s="186"/>
+      <c r="Y13" s="186"/>
+      <c r="Z13" s="186"/>
+      <c r="AA13" s="186"/>
+      <c r="AC13" s="183"/>
+      <c r="AD13" s="183"/>
+      <c r="AE13" s="183"/>
+      <c r="AF13" s="183"/>
+      <c r="AG13" s="183"/>
+      <c r="AH13" s="183"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="190"/>
-      <c r="B14" s="190"/>
-      <c r="C14" s="190"/>
-      <c r="D14" s="190"/>
-      <c r="E14" s="190"/>
-      <c r="F14" s="190"/>
-      <c r="H14" s="182"/>
-      <c r="I14" s="182"/>
-      <c r="J14" s="182"/>
-      <c r="K14" s="182"/>
-      <c r="L14" s="182"/>
-      <c r="M14" s="182"/>
-      <c r="O14" s="183"/>
-      <c r="P14" s="183"/>
-      <c r="Q14" s="183"/>
-      <c r="R14" s="183"/>
-      <c r="S14" s="183"/>
-      <c r="T14" s="183"/>
-      <c r="V14" s="184"/>
-      <c r="W14" s="184"/>
-      <c r="X14" s="184"/>
-      <c r="Y14" s="184"/>
-      <c r="Z14" s="184"/>
-      <c r="AA14" s="184"/>
-      <c r="AC14" s="185"/>
-      <c r="AD14" s="185"/>
-      <c r="AE14" s="185"/>
-      <c r="AF14" s="185"/>
-      <c r="AG14" s="185"/>
-      <c r="AH14" s="185"/>
+      <c r="A14" s="189"/>
+      <c r="B14" s="189"/>
+      <c r="C14" s="189"/>
+      <c r="D14" s="189"/>
+      <c r="E14" s="189"/>
+      <c r="F14" s="189"/>
+      <c r="H14" s="190"/>
+      <c r="I14" s="190"/>
+      <c r="J14" s="190"/>
+      <c r="K14" s="190"/>
+      <c r="L14" s="190"/>
+      <c r="M14" s="190"/>
+      <c r="O14" s="191"/>
+      <c r="P14" s="191"/>
+      <c r="Q14" s="191"/>
+      <c r="R14" s="191"/>
+      <c r="S14" s="191"/>
+      <c r="T14" s="191"/>
+      <c r="V14" s="186"/>
+      <c r="W14" s="186"/>
+      <c r="X14" s="186"/>
+      <c r="Y14" s="186"/>
+      <c r="Z14" s="186"/>
+      <c r="AA14" s="186"/>
+      <c r="AC14" s="183"/>
+      <c r="AD14" s="183"/>
+      <c r="AE14" s="183"/>
+      <c r="AF14" s="183"/>
+      <c r="AG14" s="183"/>
+      <c r="AH14" s="183"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" s="190"/>
-      <c r="B15" s="190"/>
-      <c r="C15" s="190"/>
-      <c r="D15" s="190"/>
-      <c r="E15" s="190"/>
-      <c r="F15" s="190"/>
-      <c r="H15" s="182"/>
-      <c r="I15" s="182"/>
-      <c r="J15" s="182"/>
-      <c r="K15" s="182"/>
-      <c r="L15" s="182"/>
-      <c r="M15" s="182"/>
-      <c r="O15" s="183"/>
-      <c r="P15" s="183"/>
-      <c r="Q15" s="183"/>
-      <c r="R15" s="183"/>
-      <c r="S15" s="183"/>
-      <c r="T15" s="183"/>
-      <c r="V15" s="184"/>
-      <c r="W15" s="184"/>
-      <c r="X15" s="184"/>
-      <c r="Y15" s="184"/>
-      <c r="Z15" s="184"/>
-      <c r="AA15" s="184"/>
-      <c r="AC15" s="185"/>
-      <c r="AD15" s="185"/>
-      <c r="AE15" s="185"/>
-      <c r="AF15" s="185"/>
-      <c r="AG15" s="185"/>
-      <c r="AH15" s="185"/>
+      <c r="A15" s="189"/>
+      <c r="B15" s="189"/>
+      <c r="C15" s="189"/>
+      <c r="D15" s="189"/>
+      <c r="E15" s="189"/>
+      <c r="F15" s="189"/>
+      <c r="H15" s="190"/>
+      <c r="I15" s="190"/>
+      <c r="J15" s="190"/>
+      <c r="K15" s="190"/>
+      <c r="L15" s="190"/>
+      <c r="M15" s="190"/>
+      <c r="O15" s="191"/>
+      <c r="P15" s="191"/>
+      <c r="Q15" s="191"/>
+      <c r="R15" s="191"/>
+      <c r="S15" s="191"/>
+      <c r="T15" s="191"/>
+      <c r="V15" s="186"/>
+      <c r="W15" s="186"/>
+      <c r="X15" s="186"/>
+      <c r="Y15" s="186"/>
+      <c r="Z15" s="186"/>
+      <c r="AA15" s="186"/>
+      <c r="AC15" s="183"/>
+      <c r="AD15" s="183"/>
+      <c r="AE15" s="183"/>
+      <c r="AF15" s="183"/>
+      <c r="AG15" s="183"/>
+      <c r="AH15" s="183"/>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A17" s="191" t="s">
+      <c r="A17" s="184" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="191"/>
-      <c r="C17" s="191"/>
-      <c r="D17" s="191"/>
-      <c r="E17" s="191"/>
-      <c r="F17" s="191"/>
-      <c r="H17" s="186" t="s">
+      <c r="B17" s="184"/>
+      <c r="C17" s="184"/>
+      <c r="D17" s="184"/>
+      <c r="E17" s="184"/>
+      <c r="F17" s="184"/>
+      <c r="H17" s="187" t="s">
         <v>64</v>
       </c>
-      <c r="I17" s="186"/>
-      <c r="J17" s="186"/>
-      <c r="K17" s="186"/>
-      <c r="L17" s="186"/>
-      <c r="M17" s="186"/>
-      <c r="O17" s="187" t="s">
+      <c r="I17" s="187"/>
+      <c r="J17" s="187"/>
+      <c r="K17" s="187"/>
+      <c r="L17" s="187"/>
+      <c r="M17" s="187"/>
+      <c r="O17" s="188" t="s">
         <v>64</v>
       </c>
-      <c r="P17" s="187"/>
-      <c r="Q17" s="187"/>
-      <c r="R17" s="187"/>
-      <c r="S17" s="187"/>
-      <c r="T17" s="187"/>
-      <c r="V17" s="188" t="s">
+      <c r="P17" s="188"/>
+      <c r="Q17" s="188"/>
+      <c r="R17" s="188"/>
+      <c r="S17" s="188"/>
+      <c r="T17" s="188"/>
+      <c r="V17" s="185" t="s">
         <v>64</v>
       </c>
-      <c r="W17" s="188"/>
-      <c r="X17" s="188"/>
-      <c r="Y17" s="188"/>
-      <c r="Z17" s="188"/>
-      <c r="AA17" s="188"/>
-      <c r="AC17" s="189" t="s">
+      <c r="W17" s="185"/>
+      <c r="X17" s="185"/>
+      <c r="Y17" s="185"/>
+      <c r="Z17" s="185"/>
+      <c r="AA17" s="185"/>
+      <c r="AC17" s="182" t="s">
         <v>64</v>
       </c>
-      <c r="AD17" s="189"/>
-      <c r="AE17" s="189"/>
-      <c r="AF17" s="189"/>
-      <c r="AG17" s="189"/>
-      <c r="AH17" s="189"/>
+      <c r="AD17" s="182"/>
+      <c r="AE17" s="182"/>
+      <c r="AF17" s="182"/>
+      <c r="AG17" s="182"/>
+      <c r="AH17" s="182"/>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A18" s="190" t="s">
+      <c r="A18" s="189" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="190"/>
-      <c r="C18" s="190"/>
-      <c r="D18" s="190"/>
-      <c r="E18" s="190"/>
-      <c r="F18" s="190"/>
-      <c r="H18" s="182" t="s">
+      <c r="B18" s="189"/>
+      <c r="C18" s="189"/>
+      <c r="D18" s="189"/>
+      <c r="E18" s="189"/>
+      <c r="F18" s="189"/>
+      <c r="H18" s="190" t="s">
         <v>66</v>
       </c>
-      <c r="I18" s="182"/>
-      <c r="J18" s="182"/>
-      <c r="K18" s="182"/>
-      <c r="L18" s="182"/>
-      <c r="M18" s="182"/>
-      <c r="O18" s="183" t="s">
+      <c r="I18" s="190"/>
+      <c r="J18" s="190"/>
+      <c r="K18" s="190"/>
+      <c r="L18" s="190"/>
+      <c r="M18" s="190"/>
+      <c r="O18" s="191" t="s">
         <v>65</v>
       </c>
-      <c r="P18" s="183"/>
-      <c r="Q18" s="183"/>
-      <c r="R18" s="183"/>
-      <c r="S18" s="183"/>
-      <c r="T18" s="183"/>
-      <c r="V18" s="184" t="s">
+      <c r="P18" s="191"/>
+      <c r="Q18" s="191"/>
+      <c r="R18" s="191"/>
+      <c r="S18" s="191"/>
+      <c r="T18" s="191"/>
+      <c r="V18" s="186" t="s">
         <v>65</v>
       </c>
-      <c r="W18" s="184"/>
-      <c r="X18" s="184"/>
-      <c r="Y18" s="184"/>
-      <c r="Z18" s="184"/>
-      <c r="AA18" s="184"/>
-      <c r="AC18" s="185" t="s">
+      <c r="W18" s="186"/>
+      <c r="X18" s="186"/>
+      <c r="Y18" s="186"/>
+      <c r="Z18" s="186"/>
+      <c r="AA18" s="186"/>
+      <c r="AC18" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="AD18" s="185"/>
-      <c r="AE18" s="185"/>
-      <c r="AF18" s="185"/>
-      <c r="AG18" s="185"/>
-      <c r="AH18" s="185"/>
+      <c r="AD18" s="183"/>
+      <c r="AE18" s="183"/>
+      <c r="AF18" s="183"/>
+      <c r="AG18" s="183"/>
+      <c r="AH18" s="183"/>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A19" s="190"/>
-      <c r="B19" s="190"/>
-      <c r="C19" s="190"/>
-      <c r="D19" s="190"/>
-      <c r="E19" s="190"/>
-      <c r="F19" s="190"/>
-      <c r="H19" s="182"/>
-      <c r="I19" s="182"/>
-      <c r="J19" s="182"/>
-      <c r="K19" s="182"/>
-      <c r="L19" s="182"/>
-      <c r="M19" s="182"/>
-      <c r="O19" s="183"/>
-      <c r="P19" s="183"/>
-      <c r="Q19" s="183"/>
-      <c r="R19" s="183"/>
-      <c r="S19" s="183"/>
-      <c r="T19" s="183"/>
-      <c r="V19" s="184"/>
-      <c r="W19" s="184"/>
-      <c r="X19" s="184"/>
-      <c r="Y19" s="184"/>
-      <c r="Z19" s="184"/>
-      <c r="AA19" s="184"/>
-      <c r="AC19" s="185"/>
-      <c r="AD19" s="185"/>
-      <c r="AE19" s="185"/>
-      <c r="AF19" s="185"/>
-      <c r="AG19" s="185"/>
-      <c r="AH19" s="185"/>
+      <c r="A19" s="189"/>
+      <c r="B19" s="189"/>
+      <c r="C19" s="189"/>
+      <c r="D19" s="189"/>
+      <c r="E19" s="189"/>
+      <c r="F19" s="189"/>
+      <c r="H19" s="190"/>
+      <c r="I19" s="190"/>
+      <c r="J19" s="190"/>
+      <c r="K19" s="190"/>
+      <c r="L19" s="190"/>
+      <c r="M19" s="190"/>
+      <c r="O19" s="191"/>
+      <c r="P19" s="191"/>
+      <c r="Q19" s="191"/>
+      <c r="R19" s="191"/>
+      <c r="S19" s="191"/>
+      <c r="T19" s="191"/>
+      <c r="V19" s="186"/>
+      <c r="W19" s="186"/>
+      <c r="X19" s="186"/>
+      <c r="Y19" s="186"/>
+      <c r="Z19" s="186"/>
+      <c r="AA19" s="186"/>
+      <c r="AC19" s="183"/>
+      <c r="AD19" s="183"/>
+      <c r="AE19" s="183"/>
+      <c r="AF19" s="183"/>
+      <c r="AG19" s="183"/>
+      <c r="AH19" s="183"/>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A20" s="190"/>
-      <c r="B20" s="190"/>
-      <c r="C20" s="190"/>
-      <c r="D20" s="190"/>
-      <c r="E20" s="190"/>
-      <c r="F20" s="190"/>
-      <c r="H20" s="182"/>
-      <c r="I20" s="182"/>
-      <c r="J20" s="182"/>
-      <c r="K20" s="182"/>
-      <c r="L20" s="182"/>
-      <c r="M20" s="182"/>
-      <c r="O20" s="183"/>
-      <c r="P20" s="183"/>
-      <c r="Q20" s="183"/>
-      <c r="R20" s="183"/>
-      <c r="S20" s="183"/>
-      <c r="T20" s="183"/>
-      <c r="V20" s="184"/>
-      <c r="W20" s="184"/>
-      <c r="X20" s="184"/>
-      <c r="Y20" s="184"/>
-      <c r="Z20" s="184"/>
-      <c r="AA20" s="184"/>
-      <c r="AC20" s="185"/>
-      <c r="AD20" s="185"/>
-      <c r="AE20" s="185"/>
-      <c r="AF20" s="185"/>
-      <c r="AG20" s="185"/>
-      <c r="AH20" s="185"/>
+      <c r="A20" s="189"/>
+      <c r="B20" s="189"/>
+      <c r="C20" s="189"/>
+      <c r="D20" s="189"/>
+      <c r="E20" s="189"/>
+      <c r="F20" s="189"/>
+      <c r="H20" s="190"/>
+      <c r="I20" s="190"/>
+      <c r="J20" s="190"/>
+      <c r="K20" s="190"/>
+      <c r="L20" s="190"/>
+      <c r="M20" s="190"/>
+      <c r="O20" s="191"/>
+      <c r="P20" s="191"/>
+      <c r="Q20" s="191"/>
+      <c r="R20" s="191"/>
+      <c r="S20" s="191"/>
+      <c r="T20" s="191"/>
+      <c r="V20" s="186"/>
+      <c r="W20" s="186"/>
+      <c r="X20" s="186"/>
+      <c r="Y20" s="186"/>
+      <c r="Z20" s="186"/>
+      <c r="AA20" s="186"/>
+      <c r="AC20" s="183"/>
+      <c r="AD20" s="183"/>
+      <c r="AE20" s="183"/>
+      <c r="AF20" s="183"/>
+      <c r="AG20" s="183"/>
+      <c r="AH20" s="183"/>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A21" s="190"/>
-      <c r="B21" s="190"/>
-      <c r="C21" s="190"/>
-      <c r="D21" s="190"/>
-      <c r="E21" s="190"/>
-      <c r="F21" s="190"/>
-      <c r="H21" s="182"/>
-      <c r="I21" s="182"/>
-      <c r="J21" s="182"/>
-      <c r="K21" s="182"/>
-      <c r="L21" s="182"/>
-      <c r="M21" s="182"/>
-      <c r="O21" s="183"/>
-      <c r="P21" s="183"/>
-      <c r="Q21" s="183"/>
-      <c r="R21" s="183"/>
-      <c r="S21" s="183"/>
-      <c r="T21" s="183"/>
-      <c r="V21" s="184"/>
-      <c r="W21" s="184"/>
-      <c r="X21" s="184"/>
-      <c r="Y21" s="184"/>
-      <c r="Z21" s="184"/>
-      <c r="AA21" s="184"/>
-      <c r="AC21" s="185"/>
-      <c r="AD21" s="185"/>
-      <c r="AE21" s="185"/>
-      <c r="AF21" s="185"/>
-      <c r="AG21" s="185"/>
-      <c r="AH21" s="185"/>
+      <c r="A21" s="189"/>
+      <c r="B21" s="189"/>
+      <c r="C21" s="189"/>
+      <c r="D21" s="189"/>
+      <c r="E21" s="189"/>
+      <c r="F21" s="189"/>
+      <c r="H21" s="190"/>
+      <c r="I21" s="190"/>
+      <c r="J21" s="190"/>
+      <c r="K21" s="190"/>
+      <c r="L21" s="190"/>
+      <c r="M21" s="190"/>
+      <c r="O21" s="191"/>
+      <c r="P21" s="191"/>
+      <c r="Q21" s="191"/>
+      <c r="R21" s="191"/>
+      <c r="S21" s="191"/>
+      <c r="T21" s="191"/>
+      <c r="V21" s="186"/>
+      <c r="W21" s="186"/>
+      <c r="X21" s="186"/>
+      <c r="Y21" s="186"/>
+      <c r="Z21" s="186"/>
+      <c r="AA21" s="186"/>
+      <c r="AC21" s="183"/>
+      <c r="AD21" s="183"/>
+      <c r="AE21" s="183"/>
+      <c r="AF21" s="183"/>
+      <c r="AG21" s="183"/>
+      <c r="AH21" s="183"/>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A22" s="190"/>
-      <c r="B22" s="190"/>
-      <c r="C22" s="190"/>
-      <c r="D22" s="190"/>
-      <c r="E22" s="190"/>
-      <c r="F22" s="190"/>
-      <c r="H22" s="182"/>
-      <c r="I22" s="182"/>
-      <c r="J22" s="182"/>
-      <c r="K22" s="182"/>
-      <c r="L22" s="182"/>
-      <c r="M22" s="182"/>
-      <c r="O22" s="183"/>
-      <c r="P22" s="183"/>
-      <c r="Q22" s="183"/>
-      <c r="R22" s="183"/>
-      <c r="S22" s="183"/>
-      <c r="T22" s="183"/>
-      <c r="V22" s="184"/>
-      <c r="W22" s="184"/>
-      <c r="X22" s="184"/>
-      <c r="Y22" s="184"/>
-      <c r="Z22" s="184"/>
-      <c r="AA22" s="184"/>
-      <c r="AC22" s="185"/>
-      <c r="AD22" s="185"/>
-      <c r="AE22" s="185"/>
-      <c r="AF22" s="185"/>
-      <c r="AG22" s="185"/>
-      <c r="AH22" s="185"/>
+      <c r="A22" s="189"/>
+      <c r="B22" s="189"/>
+      <c r="C22" s="189"/>
+      <c r="D22" s="189"/>
+      <c r="E22" s="189"/>
+      <c r="F22" s="189"/>
+      <c r="H22" s="190"/>
+      <c r="I22" s="190"/>
+      <c r="J22" s="190"/>
+      <c r="K22" s="190"/>
+      <c r="L22" s="190"/>
+      <c r="M22" s="190"/>
+      <c r="O22" s="191"/>
+      <c r="P22" s="191"/>
+      <c r="Q22" s="191"/>
+      <c r="R22" s="191"/>
+      <c r="S22" s="191"/>
+      <c r="T22" s="191"/>
+      <c r="V22" s="186"/>
+      <c r="W22" s="186"/>
+      <c r="X22" s="186"/>
+      <c r="Y22" s="186"/>
+      <c r="Z22" s="186"/>
+      <c r="AA22" s="186"/>
+      <c r="AC22" s="183"/>
+      <c r="AD22" s="183"/>
+      <c r="AE22" s="183"/>
+      <c r="AF22" s="183"/>
+      <c r="AG22" s="183"/>
+      <c r="AH22" s="183"/>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A24" s="191" t="s">
+      <c r="A24" s="184" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="191"/>
-      <c r="C24" s="191"/>
-      <c r="D24" s="191"/>
-      <c r="E24" s="191"/>
-      <c r="F24" s="191"/>
-      <c r="H24" s="186" t="s">
+      <c r="B24" s="184"/>
+      <c r="C24" s="184"/>
+      <c r="D24" s="184"/>
+      <c r="E24" s="184"/>
+      <c r="F24" s="184"/>
+      <c r="H24" s="187" t="s">
         <v>64</v>
       </c>
-      <c r="I24" s="186"/>
-      <c r="J24" s="186"/>
-      <c r="K24" s="186"/>
-      <c r="L24" s="186"/>
-      <c r="M24" s="186"/>
-      <c r="O24" s="187" t="s">
+      <c r="I24" s="187"/>
+      <c r="J24" s="187"/>
+      <c r="K24" s="187"/>
+      <c r="L24" s="187"/>
+      <c r="M24" s="187"/>
+      <c r="O24" s="188" t="s">
         <v>64</v>
       </c>
-      <c r="P24" s="187"/>
-      <c r="Q24" s="187"/>
-      <c r="R24" s="187"/>
-      <c r="S24" s="187"/>
-      <c r="T24" s="187"/>
-      <c r="V24" s="188" t="s">
+      <c r="P24" s="188"/>
+      <c r="Q24" s="188"/>
+      <c r="R24" s="188"/>
+      <c r="S24" s="188"/>
+      <c r="T24" s="188"/>
+      <c r="V24" s="185" t="s">
         <v>64</v>
       </c>
-      <c r="W24" s="188"/>
-      <c r="X24" s="188"/>
-      <c r="Y24" s="188"/>
-      <c r="Z24" s="188"/>
-      <c r="AA24" s="188"/>
-      <c r="AC24" s="189" t="s">
+      <c r="W24" s="185"/>
+      <c r="X24" s="185"/>
+      <c r="Y24" s="185"/>
+      <c r="Z24" s="185"/>
+      <c r="AA24" s="185"/>
+      <c r="AC24" s="182" t="s">
         <v>64</v>
       </c>
-      <c r="AD24" s="189"/>
-      <c r="AE24" s="189"/>
-      <c r="AF24" s="189"/>
-      <c r="AG24" s="189"/>
-      <c r="AH24" s="189"/>
+      <c r="AD24" s="182"/>
+      <c r="AE24" s="182"/>
+      <c r="AF24" s="182"/>
+      <c r="AG24" s="182"/>
+      <c r="AH24" s="182"/>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A25" s="190" t="s">
+      <c r="A25" s="189" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="190"/>
-      <c r="C25" s="190"/>
-      <c r="D25" s="190"/>
-      <c r="E25" s="190"/>
-      <c r="F25" s="190"/>
-      <c r="H25" s="182" t="s">
+      <c r="B25" s="189"/>
+      <c r="C25" s="189"/>
+      <c r="D25" s="189"/>
+      <c r="E25" s="189"/>
+      <c r="F25" s="189"/>
+      <c r="H25" s="190" t="s">
         <v>66</v>
       </c>
-      <c r="I25" s="182"/>
-      <c r="J25" s="182"/>
-      <c r="K25" s="182"/>
-      <c r="L25" s="182"/>
-      <c r="M25" s="182"/>
-      <c r="O25" s="183" t="s">
+      <c r="I25" s="190"/>
+      <c r="J25" s="190"/>
+      <c r="K25" s="190"/>
+      <c r="L25" s="190"/>
+      <c r="M25" s="190"/>
+      <c r="O25" s="191" t="s">
         <v>65</v>
       </c>
-      <c r="P25" s="183"/>
-      <c r="Q25" s="183"/>
-      <c r="R25" s="183"/>
-      <c r="S25" s="183"/>
-      <c r="T25" s="183"/>
-      <c r="V25" s="184" t="s">
+      <c r="P25" s="191"/>
+      <c r="Q25" s="191"/>
+      <c r="R25" s="191"/>
+      <c r="S25" s="191"/>
+      <c r="T25" s="191"/>
+      <c r="V25" s="186" t="s">
         <v>65</v>
       </c>
-      <c r="W25" s="184"/>
-      <c r="X25" s="184"/>
-      <c r="Y25" s="184"/>
-      <c r="Z25" s="184"/>
-      <c r="AA25" s="184"/>
-      <c r="AC25" s="185" t="s">
+      <c r="W25" s="186"/>
+      <c r="X25" s="186"/>
+      <c r="Y25" s="186"/>
+      <c r="Z25" s="186"/>
+      <c r="AA25" s="186"/>
+      <c r="AC25" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="AD25" s="185"/>
-      <c r="AE25" s="185"/>
-      <c r="AF25" s="185"/>
-      <c r="AG25" s="185"/>
-      <c r="AH25" s="185"/>
+      <c r="AD25" s="183"/>
+      <c r="AE25" s="183"/>
+      <c r="AF25" s="183"/>
+      <c r="AG25" s="183"/>
+      <c r="AH25" s="183"/>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A26" s="190"/>
-      <c r="B26" s="190"/>
-      <c r="C26" s="190"/>
-      <c r="D26" s="190"/>
-      <c r="E26" s="190"/>
-      <c r="F26" s="190"/>
-      <c r="H26" s="182"/>
-      <c r="I26" s="182"/>
-      <c r="J26" s="182"/>
-      <c r="K26" s="182"/>
-      <c r="L26" s="182"/>
-      <c r="M26" s="182"/>
-      <c r="O26" s="183"/>
-      <c r="P26" s="183"/>
-      <c r="Q26" s="183"/>
-      <c r="R26" s="183"/>
-      <c r="S26" s="183"/>
-      <c r="T26" s="183"/>
-      <c r="V26" s="184"/>
-      <c r="W26" s="184"/>
-      <c r="X26" s="184"/>
-      <c r="Y26" s="184"/>
-      <c r="Z26" s="184"/>
-      <c r="AA26" s="184"/>
-      <c r="AC26" s="185"/>
-      <c r="AD26" s="185"/>
-      <c r="AE26" s="185"/>
-      <c r="AF26" s="185"/>
-      <c r="AG26" s="185"/>
-      <c r="AH26" s="185"/>
+      <c r="A26" s="189"/>
+      <c r="B26" s="189"/>
+      <c r="C26" s="189"/>
+      <c r="D26" s="189"/>
+      <c r="E26" s="189"/>
+      <c r="F26" s="189"/>
+      <c r="H26" s="190"/>
+      <c r="I26" s="190"/>
+      <c r="J26" s="190"/>
+      <c r="K26" s="190"/>
+      <c r="L26" s="190"/>
+      <c r="M26" s="190"/>
+      <c r="O26" s="191"/>
+      <c r="P26" s="191"/>
+      <c r="Q26" s="191"/>
+      <c r="R26" s="191"/>
+      <c r="S26" s="191"/>
+      <c r="T26" s="191"/>
+      <c r="V26" s="186"/>
+      <c r="W26" s="186"/>
+      <c r="X26" s="186"/>
+      <c r="Y26" s="186"/>
+      <c r="Z26" s="186"/>
+      <c r="AA26" s="186"/>
+      <c r="AC26" s="183"/>
+      <c r="AD26" s="183"/>
+      <c r="AE26" s="183"/>
+      <c r="AF26" s="183"/>
+      <c r="AG26" s="183"/>
+      <c r="AH26" s="183"/>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A27" s="190"/>
-      <c r="B27" s="190"/>
-      <c r="C27" s="190"/>
-      <c r="D27" s="190"/>
-      <c r="E27" s="190"/>
-      <c r="F27" s="190"/>
-      <c r="H27" s="182"/>
-      <c r="I27" s="182"/>
-      <c r="J27" s="182"/>
-      <c r="K27" s="182"/>
-      <c r="L27" s="182"/>
-      <c r="M27" s="182"/>
-      <c r="O27" s="183"/>
-      <c r="P27" s="183"/>
-      <c r="Q27" s="183"/>
-      <c r="R27" s="183"/>
-      <c r="S27" s="183"/>
-      <c r="T27" s="183"/>
-      <c r="V27" s="184"/>
-      <c r="W27" s="184"/>
-      <c r="X27" s="184"/>
-      <c r="Y27" s="184"/>
-      <c r="Z27" s="184"/>
-      <c r="AA27" s="184"/>
-      <c r="AC27" s="185"/>
-      <c r="AD27" s="185"/>
-      <c r="AE27" s="185"/>
-      <c r="AF27" s="185"/>
-      <c r="AG27" s="185"/>
-      <c r="AH27" s="185"/>
+      <c r="A27" s="189"/>
+      <c r="B27" s="189"/>
+      <c r="C27" s="189"/>
+      <c r="D27" s="189"/>
+      <c r="E27" s="189"/>
+      <c r="F27" s="189"/>
+      <c r="H27" s="190"/>
+      <c r="I27" s="190"/>
+      <c r="J27" s="190"/>
+      <c r="K27" s="190"/>
+      <c r="L27" s="190"/>
+      <c r="M27" s="190"/>
+      <c r="O27" s="191"/>
+      <c r="P27" s="191"/>
+      <c r="Q27" s="191"/>
+      <c r="R27" s="191"/>
+      <c r="S27" s="191"/>
+      <c r="T27" s="191"/>
+      <c r="V27" s="186"/>
+      <c r="W27" s="186"/>
+      <c r="X27" s="186"/>
+      <c r="Y27" s="186"/>
+      <c r="Z27" s="186"/>
+      <c r="AA27" s="186"/>
+      <c r="AC27" s="183"/>
+      <c r="AD27" s="183"/>
+      <c r="AE27" s="183"/>
+      <c r="AF27" s="183"/>
+      <c r="AG27" s="183"/>
+      <c r="AH27" s="183"/>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A28" s="190"/>
-      <c r="B28" s="190"/>
-      <c r="C28" s="190"/>
-      <c r="D28" s="190"/>
-      <c r="E28" s="190"/>
-      <c r="F28" s="190"/>
-      <c r="H28" s="182"/>
-      <c r="I28" s="182"/>
-      <c r="J28" s="182"/>
-      <c r="K28" s="182"/>
-      <c r="L28" s="182"/>
-      <c r="M28" s="182"/>
-      <c r="O28" s="183"/>
-      <c r="P28" s="183"/>
-      <c r="Q28" s="183"/>
-      <c r="R28" s="183"/>
-      <c r="S28" s="183"/>
-      <c r="T28" s="183"/>
-      <c r="V28" s="184"/>
-      <c r="W28" s="184"/>
-      <c r="X28" s="184"/>
-      <c r="Y28" s="184"/>
-      <c r="Z28" s="184"/>
-      <c r="AA28" s="184"/>
-      <c r="AC28" s="185"/>
-      <c r="AD28" s="185"/>
-      <c r="AE28" s="185"/>
-      <c r="AF28" s="185"/>
-      <c r="AG28" s="185"/>
-      <c r="AH28" s="185"/>
+      <c r="A28" s="189"/>
+      <c r="B28" s="189"/>
+      <c r="C28" s="189"/>
+      <c r="D28" s="189"/>
+      <c r="E28" s="189"/>
+      <c r="F28" s="189"/>
+      <c r="H28" s="190"/>
+      <c r="I28" s="190"/>
+      <c r="J28" s="190"/>
+      <c r="K28" s="190"/>
+      <c r="L28" s="190"/>
+      <c r="M28" s="190"/>
+      <c r="O28" s="191"/>
+      <c r="P28" s="191"/>
+      <c r="Q28" s="191"/>
+      <c r="R28" s="191"/>
+      <c r="S28" s="191"/>
+      <c r="T28" s="191"/>
+      <c r="V28" s="186"/>
+      <c r="W28" s="186"/>
+      <c r="X28" s="186"/>
+      <c r="Y28" s="186"/>
+      <c r="Z28" s="186"/>
+      <c r="AA28" s="186"/>
+      <c r="AC28" s="183"/>
+      <c r="AD28" s="183"/>
+      <c r="AE28" s="183"/>
+      <c r="AF28" s="183"/>
+      <c r="AG28" s="183"/>
+      <c r="AH28" s="183"/>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A29" s="190"/>
-      <c r="B29" s="190"/>
-      <c r="C29" s="190"/>
-      <c r="D29" s="190"/>
-      <c r="E29" s="190"/>
-      <c r="F29" s="190"/>
-      <c r="H29" s="182"/>
-      <c r="I29" s="182"/>
-      <c r="J29" s="182"/>
-      <c r="K29" s="182"/>
-      <c r="L29" s="182"/>
-      <c r="M29" s="182"/>
-      <c r="O29" s="183"/>
-      <c r="P29" s="183"/>
-      <c r="Q29" s="183"/>
-      <c r="R29" s="183"/>
-      <c r="S29" s="183"/>
-      <c r="T29" s="183"/>
-      <c r="V29" s="184"/>
-      <c r="W29" s="184"/>
-      <c r="X29" s="184"/>
-      <c r="Y29" s="184"/>
-      <c r="Z29" s="184"/>
-      <c r="AA29" s="184"/>
-      <c r="AC29" s="185"/>
-      <c r="AD29" s="185"/>
-      <c r="AE29" s="185"/>
-      <c r="AF29" s="185"/>
-      <c r="AG29" s="185"/>
-      <c r="AH29" s="185"/>
+      <c r="A29" s="189"/>
+      <c r="B29" s="189"/>
+      <c r="C29" s="189"/>
+      <c r="D29" s="189"/>
+      <c r="E29" s="189"/>
+      <c r="F29" s="189"/>
+      <c r="H29" s="190"/>
+      <c r="I29" s="190"/>
+      <c r="J29" s="190"/>
+      <c r="K29" s="190"/>
+      <c r="L29" s="190"/>
+      <c r="M29" s="190"/>
+      <c r="O29" s="191"/>
+      <c r="P29" s="191"/>
+      <c r="Q29" s="191"/>
+      <c r="R29" s="191"/>
+      <c r="S29" s="191"/>
+      <c r="T29" s="191"/>
+      <c r="V29" s="186"/>
+      <c r="W29" s="186"/>
+      <c r="X29" s="186"/>
+      <c r="Y29" s="186"/>
+      <c r="Z29" s="186"/>
+      <c r="AA29" s="186"/>
+      <c r="AC29" s="183"/>
+      <c r="AD29" s="183"/>
+      <c r="AE29" s="183"/>
+      <c r="AF29" s="183"/>
+      <c r="AG29" s="183"/>
+      <c r="AH29" s="183"/>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A31" s="191" t="s">
+      <c r="A31" s="184" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="191"/>
-      <c r="C31" s="191"/>
-      <c r="D31" s="191"/>
-      <c r="E31" s="191"/>
-      <c r="F31" s="191"/>
-      <c r="H31" s="186" t="s">
+      <c r="B31" s="184"/>
+      <c r="C31" s="184"/>
+      <c r="D31" s="184"/>
+      <c r="E31" s="184"/>
+      <c r="F31" s="184"/>
+      <c r="H31" s="187" t="s">
         <v>64</v>
       </c>
-      <c r="I31" s="186"/>
-      <c r="J31" s="186"/>
-      <c r="K31" s="186"/>
-      <c r="L31" s="186"/>
-      <c r="M31" s="186"/>
-      <c r="O31" s="187" t="s">
+      <c r="I31" s="187"/>
+      <c r="J31" s="187"/>
+      <c r="K31" s="187"/>
+      <c r="L31" s="187"/>
+      <c r="M31" s="187"/>
+      <c r="O31" s="188" t="s">
         <v>64</v>
       </c>
-      <c r="P31" s="187"/>
-      <c r="Q31" s="187"/>
-      <c r="R31" s="187"/>
-      <c r="S31" s="187"/>
-      <c r="T31" s="187"/>
-      <c r="V31" s="188" t="s">
+      <c r="P31" s="188"/>
+      <c r="Q31" s="188"/>
+      <c r="R31" s="188"/>
+      <c r="S31" s="188"/>
+      <c r="T31" s="188"/>
+      <c r="V31" s="185" t="s">
         <v>64</v>
       </c>
-      <c r="W31" s="188"/>
-      <c r="X31" s="188"/>
-      <c r="Y31" s="188"/>
-      <c r="Z31" s="188"/>
-      <c r="AA31" s="188"/>
-      <c r="AC31" s="189" t="s">
+      <c r="W31" s="185"/>
+      <c r="X31" s="185"/>
+      <c r="Y31" s="185"/>
+      <c r="Z31" s="185"/>
+      <c r="AA31" s="185"/>
+      <c r="AC31" s="182" t="s">
         <v>64</v>
       </c>
-      <c r="AD31" s="189"/>
-      <c r="AE31" s="189"/>
-      <c r="AF31" s="189"/>
-      <c r="AG31" s="189"/>
-      <c r="AH31" s="189"/>
+      <c r="AD31" s="182"/>
+      <c r="AE31" s="182"/>
+      <c r="AF31" s="182"/>
+      <c r="AG31" s="182"/>
+      <c r="AH31" s="182"/>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A32" s="190" t="s">
+      <c r="A32" s="189" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="190"/>
-      <c r="C32" s="190"/>
-      <c r="D32" s="190"/>
-      <c r="E32" s="190"/>
-      <c r="F32" s="190"/>
-      <c r="H32" s="182" t="s">
+      <c r="B32" s="189"/>
+      <c r="C32" s="189"/>
+      <c r="D32" s="189"/>
+      <c r="E32" s="189"/>
+      <c r="F32" s="189"/>
+      <c r="H32" s="190" t="s">
         <v>66</v>
       </c>
-      <c r="I32" s="182"/>
-      <c r="J32" s="182"/>
-      <c r="K32" s="182"/>
-      <c r="L32" s="182"/>
-      <c r="M32" s="182"/>
-      <c r="O32" s="183" t="s">
+      <c r="I32" s="190"/>
+      <c r="J32" s="190"/>
+      <c r="K32" s="190"/>
+      <c r="L32" s="190"/>
+      <c r="M32" s="190"/>
+      <c r="O32" s="191" t="s">
         <v>65</v>
       </c>
-      <c r="P32" s="183"/>
-      <c r="Q32" s="183"/>
-      <c r="R32" s="183"/>
-      <c r="S32" s="183"/>
-      <c r="T32" s="183"/>
-      <c r="V32" s="184" t="s">
+      <c r="P32" s="191"/>
+      <c r="Q32" s="191"/>
+      <c r="R32" s="191"/>
+      <c r="S32" s="191"/>
+      <c r="T32" s="191"/>
+      <c r="V32" s="186" t="s">
         <v>65</v>
       </c>
-      <c r="W32" s="184"/>
-      <c r="X32" s="184"/>
-      <c r="Y32" s="184"/>
-      <c r="Z32" s="184"/>
-      <c r="AA32" s="184"/>
-      <c r="AC32" s="185" t="s">
+      <c r="W32" s="186"/>
+      <c r="X32" s="186"/>
+      <c r="Y32" s="186"/>
+      <c r="Z32" s="186"/>
+      <c r="AA32" s="186"/>
+      <c r="AC32" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="AD32" s="185"/>
-      <c r="AE32" s="185"/>
-      <c r="AF32" s="185"/>
-      <c r="AG32" s="185"/>
-      <c r="AH32" s="185"/>
+      <c r="AD32" s="183"/>
+      <c r="AE32" s="183"/>
+      <c r="AF32" s="183"/>
+      <c r="AG32" s="183"/>
+      <c r="AH32" s="183"/>
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A33" s="190"/>
-      <c r="B33" s="190"/>
-      <c r="C33" s="190"/>
-      <c r="D33" s="190"/>
-      <c r="E33" s="190"/>
-      <c r="F33" s="190"/>
-      <c r="H33" s="182"/>
-      <c r="I33" s="182"/>
-      <c r="J33" s="182"/>
-      <c r="K33" s="182"/>
-      <c r="L33" s="182"/>
-      <c r="M33" s="182"/>
-      <c r="O33" s="183"/>
-      <c r="P33" s="183"/>
-      <c r="Q33" s="183"/>
-      <c r="R33" s="183"/>
-      <c r="S33" s="183"/>
-      <c r="T33" s="183"/>
-      <c r="V33" s="184"/>
-      <c r="W33" s="184"/>
-      <c r="X33" s="184"/>
-      <c r="Y33" s="184"/>
-      <c r="Z33" s="184"/>
-      <c r="AA33" s="184"/>
-      <c r="AC33" s="185"/>
-      <c r="AD33" s="185"/>
-      <c r="AE33" s="185"/>
-      <c r="AF33" s="185"/>
-      <c r="AG33" s="185"/>
-      <c r="AH33" s="185"/>
+      <c r="A33" s="189"/>
+      <c r="B33" s="189"/>
+      <c r="C33" s="189"/>
+      <c r="D33" s="189"/>
+      <c r="E33" s="189"/>
+      <c r="F33" s="189"/>
+      <c r="H33" s="190"/>
+      <c r="I33" s="190"/>
+      <c r="J33" s="190"/>
+      <c r="K33" s="190"/>
+      <c r="L33" s="190"/>
+      <c r="M33" s="190"/>
+      <c r="O33" s="191"/>
+      <c r="P33" s="191"/>
+      <c r="Q33" s="191"/>
+      <c r="R33" s="191"/>
+      <c r="S33" s="191"/>
+      <c r="T33" s="191"/>
+      <c r="V33" s="186"/>
+      <c r="W33" s="186"/>
+      <c r="X33" s="186"/>
+      <c r="Y33" s="186"/>
+      <c r="Z33" s="186"/>
+      <c r="AA33" s="186"/>
+      <c r="AC33" s="183"/>
+      <c r="AD33" s="183"/>
+      <c r="AE33" s="183"/>
+      <c r="AF33" s="183"/>
+      <c r="AG33" s="183"/>
+      <c r="AH33" s="183"/>
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A34" s="190"/>
-      <c r="B34" s="190"/>
-      <c r="C34" s="190"/>
-      <c r="D34" s="190"/>
-      <c r="E34" s="190"/>
-      <c r="F34" s="190"/>
-      <c r="H34" s="182"/>
-      <c r="I34" s="182"/>
-      <c r="J34" s="182"/>
-      <c r="K34" s="182"/>
-      <c r="L34" s="182"/>
-      <c r="M34" s="182"/>
-      <c r="O34" s="183"/>
-      <c r="P34" s="183"/>
-      <c r="Q34" s="183"/>
-      <c r="R34" s="183"/>
-      <c r="S34" s="183"/>
-      <c r="T34" s="183"/>
-      <c r="V34" s="184"/>
-      <c r="W34" s="184"/>
-      <c r="X34" s="184"/>
-      <c r="Y34" s="184"/>
-      <c r="Z34" s="184"/>
-      <c r="AA34" s="184"/>
-      <c r="AC34" s="185"/>
-      <c r="AD34" s="185"/>
-      <c r="AE34" s="185"/>
-      <c r="AF34" s="185"/>
-      <c r="AG34" s="185"/>
-      <c r="AH34" s="185"/>
+      <c r="A34" s="189"/>
+      <c r="B34" s="189"/>
+      <c r="C34" s="189"/>
+      <c r="D34" s="189"/>
+      <c r="E34" s="189"/>
+      <c r="F34" s="189"/>
+      <c r="H34" s="190"/>
+      <c r="I34" s="190"/>
+      <c r="J34" s="190"/>
+      <c r="K34" s="190"/>
+      <c r="L34" s="190"/>
+      <c r="M34" s="190"/>
+      <c r="O34" s="191"/>
+      <c r="P34" s="191"/>
+      <c r="Q34" s="191"/>
+      <c r="R34" s="191"/>
+      <c r="S34" s="191"/>
+      <c r="T34" s="191"/>
+      <c r="V34" s="186"/>
+      <c r="W34" s="186"/>
+      <c r="X34" s="186"/>
+      <c r="Y34" s="186"/>
+      <c r="Z34" s="186"/>
+      <c r="AA34" s="186"/>
+      <c r="AC34" s="183"/>
+      <c r="AD34" s="183"/>
+      <c r="AE34" s="183"/>
+      <c r="AF34" s="183"/>
+      <c r="AG34" s="183"/>
+      <c r="AH34" s="183"/>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A35" s="190"/>
-      <c r="B35" s="190"/>
-      <c r="C35" s="190"/>
-      <c r="D35" s="190"/>
-      <c r="E35" s="190"/>
-      <c r="F35" s="190"/>
-      <c r="H35" s="182"/>
-      <c r="I35" s="182"/>
-      <c r="J35" s="182"/>
-      <c r="K35" s="182"/>
-      <c r="L35" s="182"/>
-      <c r="M35" s="182"/>
-      <c r="O35" s="183"/>
-      <c r="P35" s="183"/>
-      <c r="Q35" s="183"/>
-      <c r="R35" s="183"/>
-      <c r="S35" s="183"/>
-      <c r="T35" s="183"/>
-      <c r="V35" s="184"/>
-      <c r="W35" s="184"/>
-      <c r="X35" s="184"/>
-      <c r="Y35" s="184"/>
-      <c r="Z35" s="184"/>
-      <c r="AA35" s="184"/>
-      <c r="AC35" s="185"/>
-      <c r="AD35" s="185"/>
-      <c r="AE35" s="185"/>
-      <c r="AF35" s="185"/>
-      <c r="AG35" s="185"/>
-      <c r="AH35" s="185"/>
+      <c r="A35" s="189"/>
+      <c r="B35" s="189"/>
+      <c r="C35" s="189"/>
+      <c r="D35" s="189"/>
+      <c r="E35" s="189"/>
+      <c r="F35" s="189"/>
+      <c r="H35" s="190"/>
+      <c r="I35" s="190"/>
+      <c r="J35" s="190"/>
+      <c r="K35" s="190"/>
+      <c r="L35" s="190"/>
+      <c r="M35" s="190"/>
+      <c r="O35" s="191"/>
+      <c r="P35" s="191"/>
+      <c r="Q35" s="191"/>
+      <c r="R35" s="191"/>
+      <c r="S35" s="191"/>
+      <c r="T35" s="191"/>
+      <c r="V35" s="186"/>
+      <c r="W35" s="186"/>
+      <c r="X35" s="186"/>
+      <c r="Y35" s="186"/>
+      <c r="Z35" s="186"/>
+      <c r="AA35" s="186"/>
+      <c r="AC35" s="183"/>
+      <c r="AD35" s="183"/>
+      <c r="AE35" s="183"/>
+      <c r="AF35" s="183"/>
+      <c r="AG35" s="183"/>
+      <c r="AH35" s="183"/>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A36" s="190"/>
-      <c r="B36" s="190"/>
-      <c r="C36" s="190"/>
-      <c r="D36" s="190"/>
-      <c r="E36" s="190"/>
-      <c r="F36" s="190"/>
-      <c r="H36" s="182"/>
-      <c r="I36" s="182"/>
-      <c r="J36" s="182"/>
-      <c r="K36" s="182"/>
-      <c r="L36" s="182"/>
-      <c r="M36" s="182"/>
-      <c r="O36" s="183"/>
-      <c r="P36" s="183"/>
-      <c r="Q36" s="183"/>
-      <c r="R36" s="183"/>
-      <c r="S36" s="183"/>
-      <c r="T36" s="183"/>
-      <c r="V36" s="184"/>
-      <c r="W36" s="184"/>
-      <c r="X36" s="184"/>
-      <c r="Y36" s="184"/>
-      <c r="Z36" s="184"/>
-      <c r="AA36" s="184"/>
-      <c r="AC36" s="185"/>
-      <c r="AD36" s="185"/>
-      <c r="AE36" s="185"/>
-      <c r="AF36" s="185"/>
-      <c r="AG36" s="185"/>
-      <c r="AH36" s="185"/>
+      <c r="A36" s="189"/>
+      <c r="B36" s="189"/>
+      <c r="C36" s="189"/>
+      <c r="D36" s="189"/>
+      <c r="E36" s="189"/>
+      <c r="F36" s="189"/>
+      <c r="H36" s="190"/>
+      <c r="I36" s="190"/>
+      <c r="J36" s="190"/>
+      <c r="K36" s="190"/>
+      <c r="L36" s="190"/>
+      <c r="M36" s="190"/>
+      <c r="O36" s="191"/>
+      <c r="P36" s="191"/>
+      <c r="Q36" s="191"/>
+      <c r="R36" s="191"/>
+      <c r="S36" s="191"/>
+      <c r="T36" s="191"/>
+      <c r="V36" s="186"/>
+      <c r="W36" s="186"/>
+      <c r="X36" s="186"/>
+      <c r="Y36" s="186"/>
+      <c r="Z36" s="186"/>
+      <c r="AA36" s="186"/>
+      <c r="AC36" s="183"/>
+      <c r="AD36" s="183"/>
+      <c r="AE36" s="183"/>
+      <c r="AF36" s="183"/>
+      <c r="AG36" s="183"/>
+      <c r="AH36" s="183"/>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="AC3:AH3"/>
-    <mergeCell ref="AC4:AH8"/>
-    <mergeCell ref="AC10:AH10"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="V3:AA3"/>
-    <mergeCell ref="V4:AA8"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="O10:T10"/>
-    <mergeCell ref="V10:AA10"/>
+    <mergeCell ref="H32:M36"/>
+    <mergeCell ref="O32:T36"/>
+    <mergeCell ref="V32:AA36"/>
+    <mergeCell ref="AC32:AH36"/>
+    <mergeCell ref="H25:M29"/>
+    <mergeCell ref="O25:T29"/>
+    <mergeCell ref="V25:AA29"/>
+    <mergeCell ref="AC25:AH29"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="O31:T31"/>
+    <mergeCell ref="V31:AA31"/>
+    <mergeCell ref="AC31:AH31"/>
+    <mergeCell ref="O18:T22"/>
+    <mergeCell ref="V18:AA22"/>
+    <mergeCell ref="AC18:AH22"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="O24:T24"/>
+    <mergeCell ref="V24:AA24"/>
+    <mergeCell ref="AC24:AH24"/>
+    <mergeCell ref="V11:AA15"/>
+    <mergeCell ref="AC11:AH15"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="O17:T17"/>
+    <mergeCell ref="V17:AA17"/>
+    <mergeCell ref="AC17:AH17"/>
     <mergeCell ref="A32:F36"/>
     <mergeCell ref="H3:M3"/>
     <mergeCell ref="H4:M8"/>
@@ -36666,31 +36758,15 @@
     <mergeCell ref="H11:M15"/>
     <mergeCell ref="O11:T15"/>
     <mergeCell ref="H18:M22"/>
-    <mergeCell ref="V11:AA15"/>
-    <mergeCell ref="AC11:AH15"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="O17:T17"/>
-    <mergeCell ref="V17:AA17"/>
-    <mergeCell ref="AC17:AH17"/>
-    <mergeCell ref="O18:T22"/>
-    <mergeCell ref="V18:AA22"/>
-    <mergeCell ref="AC18:AH22"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="O24:T24"/>
-    <mergeCell ref="V24:AA24"/>
-    <mergeCell ref="AC24:AH24"/>
-    <mergeCell ref="H32:M36"/>
-    <mergeCell ref="O32:T36"/>
-    <mergeCell ref="V32:AA36"/>
-    <mergeCell ref="AC32:AH36"/>
-    <mergeCell ref="H25:M29"/>
-    <mergeCell ref="O25:T29"/>
-    <mergeCell ref="V25:AA29"/>
-    <mergeCell ref="AC25:AH29"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="O31:T31"/>
-    <mergeCell ref="V31:AA31"/>
-    <mergeCell ref="AC31:AH31"/>
+    <mergeCell ref="AC3:AH3"/>
+    <mergeCell ref="AC4:AH8"/>
+    <mergeCell ref="AC10:AH10"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="V3:AA3"/>
+    <mergeCell ref="V4:AA8"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="O10:T10"/>
+    <mergeCell ref="V10:AA10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -36829,6 +36905,11 @@
       <c r="J9" s="212"/>
       <c r="K9" s="212"/>
       <c r="L9" s="212"/>
+      <c r="N9" s="214"/>
+      <c r="O9" s="214"/>
+      <c r="P9" s="214"/>
+      <c r="Q9" s="214"/>
+      <c r="R9" s="214"/>
     </row>
     <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="203"/>
@@ -36841,6 +36922,11 @@
       <c r="J10" s="212"/>
       <c r="K10" s="212"/>
       <c r="L10" s="212"/>
+      <c r="N10" s="214"/>
+      <c r="O10" s="214"/>
+      <c r="P10" s="214"/>
+      <c r="Q10" s="214"/>
+      <c r="R10" s="214"/>
     </row>
     <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="203"/>
@@ -36853,6 +36939,11 @@
       <c r="J11" s="212"/>
       <c r="K11" s="212"/>
       <c r="L11" s="212"/>
+      <c r="N11" s="214"/>
+      <c r="O11" s="214"/>
+      <c r="P11" s="214"/>
+      <c r="Q11" s="214"/>
+      <c r="R11" s="214"/>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="203"/>
@@ -36865,6 +36956,11 @@
       <c r="J12" s="212"/>
       <c r="K12" s="212"/>
       <c r="L12" s="212"/>
+      <c r="N12" s="214"/>
+      <c r="O12" s="214"/>
+      <c r="P12" s="214"/>
+      <c r="Q12" s="214"/>
+      <c r="R12" s="214"/>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="203"/>
@@ -36877,6 +36973,11 @@
       <c r="J13" s="212"/>
       <c r="K13" s="212"/>
       <c r="L13" s="212"/>
+      <c r="N13" s="214"/>
+      <c r="O13" s="214"/>
+      <c r="P13" s="214"/>
+      <c r="Q13" s="214"/>
+      <c r="R13" s="214"/>
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="203"/>
@@ -36889,6 +36990,11 @@
       <c r="J14" s="212"/>
       <c r="K14" s="212"/>
       <c r="L14" s="212"/>
+      <c r="N14" s="214"/>
+      <c r="O14" s="214"/>
+      <c r="P14" s="214"/>
+      <c r="Q14" s="214"/>
+      <c r="R14" s="214"/>
     </row>
     <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="206"/>
@@ -36901,6 +37007,11 @@
       <c r="J15" s="212"/>
       <c r="K15" s="212"/>
       <c r="L15" s="212"/>
+      <c r="N15" s="214"/>
+      <c r="O15" s="214"/>
+      <c r="P15" s="214"/>
+      <c r="Q15" s="214"/>
+      <c r="R15" s="214"/>
     </row>
     <row r="16" spans="2:22" ht="20.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="209" t="s">
@@ -36917,6 +37028,13 @@
       <c r="J16" s="213"/>
       <c r="K16" s="213"/>
       <c r="L16" s="213"/>
+      <c r="N16" s="215" t="s">
+        <v>116</v>
+      </c>
+      <c r="O16" s="215"/>
+      <c r="P16" s="215"/>
+      <c r="Q16" s="215"/>
+      <c r="R16" s="215"/>
     </row>
     <row r="18" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="192" t="s">
@@ -36977,7 +37095,7 @@
       <c r="M21" s="173"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="B18:L20"/>
     <mergeCell ref="B4:V4"/>
     <mergeCell ref="C5:V5"/>
@@ -36987,6 +37105,8 @@
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="H9:L15"/>
     <mergeCell ref="H16:L16"/>
+    <mergeCell ref="N9:R15"/>
+    <mergeCell ref="N16:R16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -36999,7 +37119,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37382,21 +37502,21 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="214" t="s">
+      <c r="J7" s="216" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="215"/>
-      <c r="L7" s="215"/>
-      <c r="M7" s="215"/>
-      <c r="N7" s="216"/>
+      <c r="K7" s="217"/>
+      <c r="L7" s="217"/>
+      <c r="M7" s="217"/>
+      <c r="N7" s="218"/>
       <c r="O7" s="9"/>
       <c r="P7" s="12"/>
-      <c r="Q7" s="217" t="s">
+      <c r="Q7" s="219" t="s">
         <v>24</v>
       </c>
-      <c r="R7" s="218"/>
-      <c r="S7" s="218"/>
-      <c r="T7" s="219"/>
+      <c r="R7" s="220"/>
+      <c r="S7" s="220"/>
+      <c r="T7" s="221"/>
       <c r="U7" s="4"/>
       <c r="V7" s="8" t="s">
         <v>50</v>
@@ -37412,17 +37532,17 @@
       <c r="AC7" s="13"/>
       <c r="AD7" s="11"/>
       <c r="AE7" s="5"/>
-      <c r="AF7" s="214" t="s">
+      <c r="AF7" s="216" t="s">
         <v>52</v>
       </c>
-      <c r="AG7" s="218"/>
-      <c r="AH7" s="218"/>
-      <c r="AI7" s="218"/>
-      <c r="AJ7" s="218"/>
-      <c r="AK7" s="218"/>
-      <c r="AL7" s="218"/>
-      <c r="AM7" s="218"/>
-      <c r="AN7" s="218"/>
+      <c r="AG7" s="220"/>
+      <c r="AH7" s="220"/>
+      <c r="AI7" s="220"/>
+      <c r="AJ7" s="220"/>
+      <c r="AK7" s="220"/>
+      <c r="AL7" s="220"/>
+      <c r="AM7" s="220"/>
+      <c r="AN7" s="220"/>
       <c r="AO7" s="11"/>
       <c r="AP7" s="11"/>
       <c r="AQ7" s="11"/>
@@ -37608,15 +37728,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100065FB0D312CA5248B20C1FB505595AC8" ma:contentTypeVersion="23" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="4f7a8c67b87e371bcf13ffc792a60c3d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="37733d2e-ea70-4519-86c9-46ac9bf5a057" xmlns:ns3="d941cd37-1e6b-493f-add9-e5fae16f2df6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ec0750c6ba13a701a41ea22f79b1789" ns2:_="" ns3:_="">
     <xsd:import namespace="37733d2e-ea70-4519-86c9-46ac9bf5a057"/>
@@ -37984,6 +38095,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -38004,14 +38124,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7327DEDC-BB23-41C5-B379-88E746B31711}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -38026,6 +38138,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4A34E49-7289-4AEA-9593-4F55E04ADB10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>